<commit_message>
bugfixes: import auf "kinderbetreuung" (auch für das logging), plots.R ebenfalls sourcen, examples für plot_summary_teil_1 vervollständigt, tags für alle fragen
</commit_message>
<xml_diff>
--- a/inst/shiny-apps/vsim/data/vsim_question_lists_kinderbetreuung.xlsx
+++ b/inst/shiny-apps/vsim/data/vsim_question_lists_kinderbetreuung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10923"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianschmid/Documents/R/vsim/inst/shiny-apps/vsim/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942614F2-3B94-5344-ACAD-47B1D2916DBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B5E83A-DD57-A146-89BE-E5CD7E26D07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
   </bookViews>
   <sheets>
     <sheet name="QAGlist_Teil1" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="154">
   <si>
     <t>Qnum</t>
   </si>
@@ -489,6 +489,18 @@
   </si>
   <si>
     <t>für andere Tätigkeiten</t>
+  </si>
+  <si>
+    <t>Arbeit</t>
+  </si>
+  <si>
+    <t>Haushalt &amp; Selbstsorge</t>
+  </si>
+  <si>
+    <t>Soziales Umfeld</t>
+  </si>
+  <si>
+    <t>Arbeit,Haushalt &amp; Selbstsorge</t>
   </si>
 </sst>
 </file>
@@ -554,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -562,7 +574,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -570,6 +581,36 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -686,36 +727,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -733,19 +744,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9A4626D1-B7A1-4A0E-9ABD-F1802EEF4B4A}" name="Qlist_Teil1" displayName="Qlist_Teil1" ref="A1:M33" totalsRowShown="0">
   <autoFilter ref="A1:M33" xr:uid="{63A3C723-9C80-47B3-B07E-C2015D435A2D}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6833DAB1-3042-428C-936F-D4BF6D9DD972}" name="Qnum" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{68ACE6E4-2458-484E-B5F0-6043D861F09A}" name="Question" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{AC5C841C-1944-4079-B15A-B674D389AD3B}" name="Answer1" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{D9A448EB-5507-4F2F-8169-E03A078A2E00}" name="Answer2" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{F5AE864E-E78B-48B0-8119-6488E57CDEC2}" name="Answer3" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{820B5DC6-DC55-4530-8199-59BBF110D652}" name="Answer4" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{BE2656F8-6B4A-4CA5-8BCE-B4A76AE8B405}" name="Answer5" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{CA09BC99-FE00-46ED-A0B4-6FE845E2BCD8}" name="Answer_given" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{CF4BC041-1816-4FFC-B75C-557A93F1E5A5}" name="Gap1" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{67DE16B3-7423-47B2-9C5A-1D73877CF226}" name="Indikator1" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{B8338369-1A8C-4167-9471-0FB565CCC681}" name="Gap2" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{B5431A50-5B31-446D-9AB0-E942AC0F72D0}" name="Indikator2" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{2652274F-4F9A-4B4F-BF81-94518D6632CD}" name="Gap1_type" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6833DAB1-3042-428C-936F-D4BF6D9DD972}" name="Qnum" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{68ACE6E4-2458-484E-B5F0-6043D861F09A}" name="Question" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{AC5C841C-1944-4079-B15A-B674D389AD3B}" name="Answer1" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{D9A448EB-5507-4F2F-8169-E03A078A2E00}" name="Answer2" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{F5AE864E-E78B-48B0-8119-6488E57CDEC2}" name="Answer3" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{820B5DC6-DC55-4530-8199-59BBF110D652}" name="Answer4" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{BE2656F8-6B4A-4CA5-8BCE-B4A76AE8B405}" name="Answer5" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{CA09BC99-FE00-46ED-A0B4-6FE845E2BCD8}" name="Answer_given" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{CF4BC041-1816-4FFC-B75C-557A93F1E5A5}" name="Gap1" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{67DE16B3-7423-47B2-9C5A-1D73877CF226}" name="Indikator1" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{B8338369-1A8C-4167-9471-0FB565CCC681}" name="Gap2" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{B5431A50-5B31-446D-9AB0-E942AC0F72D0}" name="Indikator2" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{2652274F-4F9A-4B4F-BF81-94518D6632CD}" name="Gap1_type" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -756,9 +767,9 @@
   <autoFilter ref="A1:D13" xr:uid="{69F604FC-BD72-45D2-A09E-B8F95767F925}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{41369CAF-6A0E-4C18-B180-87ACD091F8AB}" name="Qnum"/>
-    <tableColumn id="2" xr3:uid="{5E044037-C44B-46B9-8C96-3D4D32F4B88B}" name="Question" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{F9B3C5A3-3257-4569-B396-F7CE4ED9D5D4}" name="Massnahme" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{A39A07FB-44C9-43C4-8124-5CD907E9A451}" name="Column1" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{5E044037-C44B-46B9-8C96-3D4D32F4B88B}" name="Question" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{F9B3C5A3-3257-4569-B396-F7CE4ED9D5D4}" name="Massnahme" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A39A07FB-44C9-43C4-8124-5CD907E9A451}" name="Column1" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -769,7 +780,7 @@
   <autoFilter ref="A1:B7" xr:uid="{811BCABA-8AC9-47EE-B25C-AC015A6BA529}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{14CC1A9D-6C2A-40D3-A4C6-6D9D97EBCB10}" name="Qnum"/>
-    <tableColumn id="2" xr3:uid="{92BB0A0A-CB23-4959-8A93-EE395CEC4FCA}" name="Question" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{92BB0A0A-CB23-4959-8A93-EE395CEC4FCA}" name="Question" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -780,12 +791,12 @@
   <autoFilter ref="A1:G9" xr:uid="{B8CF705B-8783-48EC-88AB-BE7C260D7C0A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{C508B75E-57FF-477F-8287-3E84B131A9B9}" name="Qnum"/>
-    <tableColumn id="2" xr3:uid="{17968811-FCD2-48AB-9942-48F47827B77F}" name="Question" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{E3FC7B88-9E8D-4955-B37F-8995D4F40263}" name="Answer1" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{8ECF35DD-CB27-42A7-941E-01EADD3EC580}" name="Answer2" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{4219D505-2698-41AC-8808-9C5E297C56C5}" name="Answer3" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{EE17B9AD-B775-4DA2-B745-B64917ADD63C}" name="Answer4" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{770D580F-CBC1-478A-B1FA-45EF095D5BE1}" name="Answer5" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{17968811-FCD2-48AB-9942-48F47827B77F}" name="Question" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{E3FC7B88-9E8D-4955-B37F-8995D4F40263}" name="Answer1" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{8ECF35DD-CB27-42A7-941E-01EADD3EC580}" name="Answer2" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{4219D505-2698-41AC-8808-9C5E297C56C5}" name="Answer3" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{EE17B9AD-B775-4DA2-B745-B64917ADD63C}" name="Answer4" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{770D580F-CBC1-478A-B1FA-45EF095D5BE1}" name="Answer5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1090,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F2727F-E159-4B39-B30A-A10ACC8F5533}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="H5" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1131,7 +1142,7 @@
       <c r="G1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>124</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -1170,7 +1181,7 @@
       <c r="G2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="5" t="s">
         <v>14</v>
       </c>
@@ -1183,7 +1194,9 @@
       <c r="L2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="7"/>
+      <c r="M2" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -1205,7 +1218,7 @@
       <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1218,7 +1231,9 @@
       <c r="L3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="7"/>
+      <c r="M3" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -1240,7 +1255,7 @@
       <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1253,7 +1268,9 @@
       <c r="L4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="7"/>
+      <c r="M4" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -1275,7 +1292,7 @@
       <c r="G5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="5" t="s">
         <v>22</v>
       </c>
@@ -1288,7 +1305,9 @@
       <c r="L5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="7"/>
+      <c r="M5" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
@@ -1310,7 +1329,7 @@
       <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1323,7 +1342,9 @@
       <c r="L6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="7"/>
+      <c r="M6" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -1345,7 +1366,7 @@
       <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="5" t="s">
         <v>22</v>
       </c>
@@ -1358,7 +1379,9 @@
       <c r="L7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="7"/>
+      <c r="M7" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
@@ -1380,7 +1403,7 @@
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1393,7 +1416,9 @@
       <c r="L8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="7"/>
+      <c r="M8" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
@@ -1415,7 +1440,7 @@
       <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="5" t="s">
         <v>25</v>
       </c>
@@ -1428,7 +1453,9 @@
       <c r="L9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="7"/>
+      <c r="M9" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
@@ -1450,7 +1477,7 @@
       <c r="G10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="5" t="s">
         <v>25</v>
       </c>
@@ -1463,7 +1490,9 @@
       <c r="L10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="7"/>
+      <c r="M10" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
@@ -1483,7 +1512,7 @@
       <c r="G11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1496,7 +1525,9 @@
       <c r="L11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="7"/>
+      <c r="M11" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
@@ -1516,7 +1547,7 @@
       <c r="G12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
         <v>20</v>
       </c>
@@ -1529,7 +1560,9 @@
       <c r="L12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="7"/>
+      <c r="M12" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
@@ -1549,7 +1582,7 @@
       <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1562,7 +1595,9 @@
       <c r="L13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="M13" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -1582,7 +1617,7 @@
         <v>83</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
         <v>138</v>
       </c>
@@ -1591,7 +1626,9 @@
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="7"/>
+      <c r="M14" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
@@ -1611,7 +1648,7 @@
         <v>83</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="8"/>
       <c r="I15" s="5" t="s">
         <v>140</v>
       </c>
@@ -1620,7 +1657,9 @@
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="7"/>
+      <c r="M15" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
@@ -1640,7 +1679,7 @@
         <v>83</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="9"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="5" t="s">
         <v>142</v>
       </c>
@@ -1649,7 +1688,9 @@
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="7"/>
+      <c r="M16" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
@@ -1671,7 +1712,7 @@
       <c r="G17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="9"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="5" t="s">
         <v>28</v>
       </c>
@@ -1684,7 +1725,9 @@
       <c r="L17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="7"/>
+      <c r="M17" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
@@ -1706,7 +1749,7 @@
       <c r="G18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="9"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1719,7 +1762,9 @@
       <c r="L18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M18" s="7"/>
+      <c r="M18" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
@@ -1741,7 +1786,7 @@
       <c r="G19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="5" t="s">
         <v>33</v>
       </c>
@@ -1754,7 +1799,9 @@
       <c r="L19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M19" s="7"/>
+      <c r="M19" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
@@ -1776,7 +1823,7 @@
       <c r="G20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="9"/>
+      <c r="H20" s="8"/>
       <c r="I20" s="5" t="s">
         <v>34</v>
       </c>
@@ -1789,7 +1836,9 @@
       <c r="L20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M20" s="7"/>
+      <c r="M20" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
@@ -1811,7 +1860,7 @@
       <c r="G21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="5" t="s">
         <v>34</v>
       </c>
@@ -1824,7 +1873,9 @@
       <c r="L21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="7"/>
+      <c r="M21" s="6" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
@@ -1846,7 +1897,7 @@
       <c r="G22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="9"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="5" t="s">
         <v>33</v>
       </c>
@@ -1859,7 +1910,9 @@
       <c r="L22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M22" s="7"/>
+      <c r="M22" s="6" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
@@ -1881,7 +1934,7 @@
       <c r="G23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="5" t="s">
         <v>35</v>
       </c>
@@ -1894,7 +1947,9 @@
       <c r="L23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M23" s="7"/>
+      <c r="M23" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
@@ -1916,7 +1971,7 @@
       <c r="G24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="9"/>
+      <c r="H24" s="8"/>
       <c r="I24" s="5" t="s">
         <v>31</v>
       </c>
@@ -1929,7 +1984,9 @@
       <c r="L24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M24" s="7"/>
+      <c r="M24" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
@@ -1951,7 +2008,7 @@
       <c r="G25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="9"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="5" t="s">
         <v>36</v>
       </c>
@@ -1964,7 +2021,9 @@
       <c r="L25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M25" s="7"/>
+      <c r="M25" s="6" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
@@ -1986,7 +2045,7 @@
       <c r="G26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="9"/>
+      <c r="H26" s="8"/>
       <c r="I26" s="5" t="s">
         <v>35</v>
       </c>
@@ -1999,7 +2058,9 @@
       <c r="L26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M26" s="7"/>
+      <c r="M26" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
@@ -2019,7 +2080,7 @@
         <v>83</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="9"/>
+      <c r="H27" s="8"/>
       <c r="I27" s="5" t="s">
         <v>37</v>
       </c>
@@ -2028,7 +2089,9 @@
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="7"/>
+      <c r="M27" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
@@ -2050,7 +2113,7 @@
       <c r="G28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="9"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="5" t="s">
         <v>31</v>
       </c>
@@ -2063,7 +2126,9 @@
       <c r="L28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M28" s="7"/>
+      <c r="M28" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
@@ -2085,7 +2150,7 @@
       <c r="G29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="9"/>
+      <c r="H29" s="8"/>
       <c r="I29" s="5" t="s">
         <v>38</v>
       </c>
@@ -2098,7 +2163,9 @@
       <c r="L29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M29" s="7"/>
+      <c r="M29" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
@@ -2120,7 +2187,7 @@
       <c r="G30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="9"/>
+      <c r="H30" s="8"/>
       <c r="I30" s="5" t="s">
         <v>148</v>
       </c>
@@ -2133,7 +2200,9 @@
       <c r="L30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M30" s="7"/>
+      <c r="M30" s="6" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
@@ -2155,7 +2224,7 @@
       <c r="G31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="9"/>
+      <c r="H31" s="8"/>
       <c r="I31" s="5" t="s">
         <v>39</v>
       </c>
@@ -2168,7 +2237,9 @@
       <c r="L31" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M31" s="7"/>
+      <c r="M31" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
@@ -2190,7 +2261,7 @@
       <c r="G32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="9"/>
+      <c r="H32" s="8"/>
       <c r="I32" s="5" t="s">
         <v>40</v>
       </c>
@@ -2203,7 +2274,9 @@
       <c r="L32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M32" s="7"/>
+      <c r="M32" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
@@ -2225,7 +2298,7 @@
       <c r="G33" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="9"/>
+      <c r="H33" s="8"/>
       <c r="I33" s="5" t="s">
         <v>41</v>
       </c>
@@ -2238,7 +2311,9 @@
       <c r="L33" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M33" s="7"/>
+      <c r="M33" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2459,7 +2534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF4EA90-0C81-4B25-A330-594E7D4EAFFD}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Anpassung der Fragen mit Myriel
</commit_message>
<xml_diff>
--- a/inst/shiny-apps/vsim/data/vsim_question_lists_kinderbetreuung.xlsx
+++ b/inst/shiny-apps/vsim/data/vsim_question_lists_kinderbetreuung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianschmid/Documents/R/vsim/inst/shiny-apps/vsim/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B5E83A-DD57-A146-89BE-E5CD7E26D07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D238A41-5673-9A45-9701-B85A998CCD39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="150">
   <si>
     <t>Qnum</t>
   </si>
@@ -56,21 +56,12 @@
     <t>Nein, ich möchte gern weniger Zeit dafür verwenden</t>
   </si>
   <si>
-    <t>Finden Sie es in Ordnung, wie viel Zeit Sie pro Woche für Hausarbeiten wie Putzen, Kochen, Reparieren, Gartenarbeit, Zahlungen, Einkaufen, Waschen etc. verwenden?</t>
-  </si>
-  <si>
-    <t>Finden Sie es in Ordnung, wie viel Zeit Sie pro Woche für die Kinderbetreuung verwenden?</t>
-  </si>
-  <si>
     <t>Ich verbringe genügend Zeit mit meinem/meinen Kind(ern), um zu spielen, zu basteln, Sport zu treiben, zu lesen oder Ähnliches zu unternehmen.</t>
   </si>
   <si>
     <t>Ich verbringe genügend Zeit zu zweit mit meiner Partnerin/meinem Partner.</t>
   </si>
   <si>
-    <t>Ich fühle mich während des Home Office belastet, weil oftmals private Aufgaben dazwischen kommen.</t>
-  </si>
-  <si>
     <t>Gap1</t>
   </si>
   <si>
@@ -122,18 +113,12 @@
     <t>In meiner Freizeit verbringe ich genügend Zeit mit Freunden/Verwandten oder in Vereinen, Sportclubs und/oder Ähnlichem.</t>
   </si>
   <si>
-    <t>Ich bin zufrieden mit meinen aktuellen Möglichkeiten zur Karriereentwicklung (Mein Arbeitgeber unterstützt mich darin, mich weiterzuentwickeln oder weiterzubilden und meine familiäre Situation lässt dies zu).</t>
-  </si>
-  <si>
     <t>Unzufriedenheit mit der Karriereentwicklung</t>
   </si>
   <si>
     <t>Belastung: Schwierigkeiten abzuschalten</t>
   </si>
   <si>
-    <t>Ich fühle mich oft belastet, weil die Organisation der Vereinbarkeit kompliziert ist (z.B. Kind ist krank, Kinder von der KITA abholen, Hausarbeiten, Einkäufe etc.)</t>
-  </si>
-  <si>
     <t>Belastung: Häufiges Hin- und Herschalten zwischen Privatem und Beruflichem (Switchen)</t>
   </si>
   <si>
@@ -296,30 +281,6 @@
     <t>In meiner Freizeit verbringe ich genügend Zeit mit Aktivitäten wie Wandern, Spazieren, Velofahren, Lesen, Fernsehen, Ausruhen und/oder Ähnlichem.</t>
   </si>
   <si>
-    <t>Ich fühle mich oft belastet, weil ich in meiner Freizeit viele Besorgungen, Termine, etc. erledigen muss, dies aber oftmals nicht in der gegebenen Zeit schaffe.</t>
-  </si>
-  <si>
-    <t>Ich habe oft ein schlechtes Gewissen, weil ich aufgrund von privaten Verpflichtungen die Erwartungen meines Arbeitgebers oftmals nicht erfüllen kann.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich habe oft ein schlechtes Gewissen, weil ich aufgrund von beruflichen Verpflichtungen meine Erwartungen bezüglich Haushalt oder Kinderbetreuung nicht erfüllen kann.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich fühle mich oft belastet, weil ich während der Arbeit oder in der Freizeit oftmals verschiedene Dinge gleichzeitig erledigen muss. </t>
-  </si>
-  <si>
-    <t>Ich fühle mich oft belastet, weil ich während der Arbeit oftmals auch privaten Verpflichtungen nachkommen muss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich fühle mich oft belastet, weil ich zu Hause oftmals auch beruflichen Verpflichtungen nachkommen muss.  </t>
-  </si>
-  <si>
-    <t>Ich fühle mich oft belastet, weil die zeitliche Beanspruchung von Arbeit und privaten Verpflichtungen insgesamt zu hoch ist.</t>
-  </si>
-  <si>
-    <t>Ich fühle mich oft belastet, weil die finanzielle Situation in meinem Haushalt angespannt ist.</t>
-  </si>
-  <si>
     <t>Möchten Sie einplanen, die Zuständigkeiten für das Geldverdienen in Ihrem Haushalt neu zu verhandeln?</t>
   </si>
   <si>
@@ -419,24 +380,6 @@
     <t>Gap1_type</t>
   </si>
   <si>
-    <t>viel mehr Zeit verwenden.</t>
-  </si>
-  <si>
-    <t>ein bisschen mehr Zeit verwenden.</t>
-  </si>
-  <si>
-    <t>gleich viel Zeit verwenden.</t>
-  </si>
-  <si>
-    <t>ein bisschen weniger Zeit verwenden.</t>
-  </si>
-  <si>
-    <t>viel weniger Zeit aufwenden.</t>
-  </si>
-  <si>
-    <t>Finden Sie es in Ordnung, wie viel Zeit Sie pro Woche für die Erwerbsarbeit (inkl. Pendeln, Übernachtungen, Pausen und Mittagszeiten) aufbringen?&lt;p&gt;Ich möchte gerne..&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Wie häufig erledigen Sie während der Arbeitszeit zwischendurch oder zu Randzeiten private Verpflichtungen (z.B. Einkäufe erledigen, Mittagessen zubereiten, Versorgen von Kindern, Pflege von Angehörigen)?</t>
   </si>
   <si>
@@ -458,9 +401,6 @@
     <t>Unzufriedenheit mit den Arbeitsinhalten</t>
   </si>
   <si>
-    <t>Ich fühle mich in meiner Arbeit wertgeschätzt durch meine Kolleg*innen, Vorgesetzten und die Firmenleitung</t>
-  </si>
-  <si>
     <t>Unzufriedenheit mit der Wertschätzung</t>
   </si>
   <si>
@@ -473,18 +413,9 @@
     <t>Ich fühle mich belastet, weil ich meine Aufgaben bei der Arbeit unter hohem Zeitdruck erledigen muss.</t>
   </si>
   <si>
-    <t>Ich fühle mich belastet, weil ich ausserhalb meiner Arbeitszeit  oftmals auch beruflichen Verpflichtungen nachkommen muss und deshalb zu wenig Zeit für andere Tätigkeiten habe.</t>
-  </si>
-  <si>
     <t>Ich empfinde meine berufliche Zukunft als ungewiss und fühle mich oft dadurch belastet.</t>
   </si>
   <si>
-    <t>Ich fühle mit oft belastet, weil ich mich körperlich nicht gesund fühle.</t>
-  </si>
-  <si>
-    <t>Ich fühle mit oft belastet, weil es mir emotional nicht gut geht.</t>
-  </si>
-  <si>
     <t>Belastung: Berufliche Zukunft</t>
   </si>
   <si>
@@ -501,6 +432,63 @@
   </si>
   <si>
     <t>Arbeit,Haushalt &amp; Selbstsorge</t>
+  </si>
+  <si>
+    <t>Finden Sie es in Ordnung, wie viel Zeit Sie pro Woche für die Kinderbetreuung im engeren Sinne (Hausaufgaben erledigen, Essen zubereiten etc.) aufwenden?</t>
+  </si>
+  <si>
+    <t>Ich fühle mich in meiner Arbeit wertgeschätzt durch meine Kolleg_innen, Vorgesetzten und die Firmenleitung</t>
+  </si>
+  <si>
+    <t>Ich bin zufrieden mit meinen aktuellen Möglichkeiten zur Karriereentwicklung.</t>
+  </si>
+  <si>
+    <t>Ich fühle mich belastet, weil ich in meiner Freizeit viele Besorgungen, Termine, etc. erledigen muss, dies aber oft nicht in der gegebenen Zeit schaffe.</t>
+  </si>
+  <si>
+    <t>Ich habe ein schlechtes Gewissen, weil ich aufgrund von privaten Verpflichtungen die Erwartungen meines Arbeitgebers und/oder meiner Arbeitskolleg_innen oft nicht erfüllen kann.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich habe ein schlechtes Gewissen, weil ich aufgrund von beruflichen Verpflichtungen meine Erwartungen bezüglich Haushalt oder Kinderbetreuung nicht erfüllen kann.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich fühle mich belastet, weil ich während der Arbeit oder in der Freizeit oft verschiedene Dinge gleichzeitig erledigen muss. </t>
+  </si>
+  <si>
+    <t>Ich fühle mich belastet, weil ich während der Arbeit oft auch privaten Verpflichtungen nachkommen muss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich fühle mich belastet, weil ich zu Hause oft auch beruflichen Verpflichtungen nachkommen muss.  </t>
+  </si>
+  <si>
+    <t>Ich fühle mich belastet, weil ich ausserhalb meiner Arbeitszeit oft auch beruflichen Verpflichtungen nachkommen muss und deshalb zu wenig Zeit für andere Tätigkeiten habe.</t>
+  </si>
+  <si>
+    <t>Ich fühle mich während des Home Office belastet, weil oft private Aufgaben dazwischen kommen.</t>
+  </si>
+  <si>
+    <t>Ich fühle mich belastet, weil die zeitliche Beanspruchung von Arbeit und privaten Verpflichtungen insgesamt zu hoch ist.</t>
+  </si>
+  <si>
+    <t>Ich fühle mich belastet, weil die Organisation der Vereinbarkeit oft kompliziert ist (z.B. Kind ist krank, Kinder von der KITA abholen, Hausarbeiten, Einkäufe etc.)</t>
+  </si>
+  <si>
+    <t>Ich fühle mich belastet, weil die finanzielle Situation in meinem Haushalt angespannt ist.</t>
+  </si>
+  <si>
+    <t>Ich fühle mich belastet, weil ich mich körperlich oft nicht gesund fühle.</t>
+  </si>
+  <si>
+    <t>Ich fühle mich belastet, weil es mir emotional oft nicht gut geht.</t>
+  </si>
+  <si>
+    <t>Arbeit, Haushalt &amp; Selbstsorge</t>
+  </si>
+  <si>
+    <t>Finden Sie es in Ordnung, wie viel Zeit Sie pro Woche für die Erwerbsarbeit (inkl. Pendeln, Übernachtungen, Pausen und Mittagszeiten) aufwenden?</t>
+  </si>
+  <si>
+    <t>Finden Sie es in Ordnung, wie viel Zeit Sie pro Woche für Hausarbeiten (wie Putzen, Kochen, Reparieren, Gartenarbeit, Zahlungen, Einkaufen, Waschen etc.) aufwenden?</t>
   </si>
 </sst>
 </file>
@@ -776,8 +764,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6155BF54-C55B-4CA3-AA2D-6B56FF8A665A}" name="QInputlist_Teil2b" displayName="QInputlist_Teil2b" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{811BCABA-8AC9-47EE-B25C-AC015A6BA529}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6155BF54-C55B-4CA3-AA2D-6B56FF8A665A}" name="QInputlist_Teil2b" displayName="QInputlist_Teil2b" ref="A1:B8" totalsRowShown="0">
+  <autoFilter ref="A1:B8" xr:uid="{811BCABA-8AC9-47EE-B25C-AC015A6BA529}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{14CC1A9D-6C2A-40D3-A4C6-6D9D97EBCB10}" name="Qnum"/>
     <tableColumn id="2" xr3:uid="{92BB0A0A-CB23-4959-8A93-EE395CEC4FCA}" name="Question" dataDxfId="6"/>
@@ -1101,22 +1089,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F2727F-E159-4B39-B30A-A10ACC8F5533}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="158.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="117" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="9" width="48" customWidth="1"/>
-    <col min="10" max="10" width="72.83203125" customWidth="1"/>
+    <col min="9" max="9" width="41.83203125" customWidth="1"/>
+    <col min="10" max="10" width="70.5" customWidth="1"/>
+    <col min="11" max="12" width="10.83203125" customWidth="1"/>
     <col min="13" max="13" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1128,259 +1117,251 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="M1" s="6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>127</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>130</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="8"/>
       <c r="I2" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1389,344 +1370,338 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>152</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>151</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>151</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="6" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="8"/>
       <c r="I15" s="5" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="6" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="8"/>
       <c r="I16" s="5" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="6" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1735,584 +1710,584 @@
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="8"/>
       <c r="I27" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
-        <v>30</v>
+        <v>143</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="5" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="3" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2348,10 +2323,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2359,13 +2334,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2373,13 +2348,13 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2387,13 +2362,13 @@
         <v>2.1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2401,13 +2376,13 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2415,13 +2390,13 @@
         <v>3.1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2429,13 +2404,13 @@
         <v>3.2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2443,13 +2418,13 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2457,13 +2432,13 @@
         <v>4.2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2471,13 +2446,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2485,13 +2460,13 @@
         <v>5.2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2499,13 +2474,13 @@
         <v>6.1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2513,13 +2488,13 @@
         <v>6.2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2532,10 +2507,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF4EA90-0C81-4B25-A330-594E7D4EAFFD}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2557,7 +2532,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2565,7 +2540,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2573,7 +2548,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2581,7 +2556,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2589,7 +2564,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2597,8 +2572,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2634,19 +2612,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2654,22 +2632,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2677,22 +2655,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2700,22 +2678,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2723,22 +2701,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2746,22 +2724,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2769,22 +2747,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2792,22 +2770,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2815,22 +2793,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfix: vsim_question_lists_kinderbetreuung.xlsx, bei Frage 1 falsche Indikatoren definiert
</commit_message>
<xml_diff>
--- a/inst/shiny-apps/vsim/data/vsim_question_lists_kinderbetreuung.xlsx
+++ b/inst/shiny-apps/vsim/data/vsim_question_lists_kinderbetreuung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianschmid/Documents/R/vsim/inst/shiny-apps/vsim/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D238A41-5673-9A45-9701-B85A998CCD39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE01E6E0-F8CF-514A-BCB1-17CCF693B719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
   </bookViews>
   <sheets>
     <sheet name="QAGlist_Teil1" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="149">
   <si>
     <t>Qnum</t>
   </si>
@@ -390,9 +390,6 @@
   </si>
   <si>
     <t>Wie häufig führen private Verpflichtungen (z.B. Einkäufe erledigen, Mittagessen zubereiten, Versorgen von Kindern, Pflege von Angehörigen) dazu, dass Sie Ihren Arbeitsplatz früher verlassen bzw. später eintreffen?</t>
-  </si>
-  <si>
-    <t>mehr</t>
   </si>
   <si>
     <t>Ich finde meine Arbeit spannend und relevant und meine Fähigkeiten entsprechen den Arbeitsanforderungen.</t>
@@ -1089,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F2727F-E159-4B39-B30A-A10ACC8F5533}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1153,7 +1150,7 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>71</v>
@@ -1171,7 +1168,7 @@
         <v>11</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>13</v>
@@ -1180,13 +1177,13 @@
         <v>13</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>71</v>
@@ -1215,13 +1212,13 @@
         <v>13</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>71</v>
@@ -1250,7 +1247,7 @@
         <v>13</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1287,7 +1284,7 @@
         <v>13</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1324,7 +1321,7 @@
         <v>13</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1361,7 +1358,7 @@
         <v>13</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1398,7 +1395,7 @@
         <v>13</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1435,7 +1432,7 @@
         <v>13</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1472,7 +1469,7 @@
         <v>13</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1577,7 +1574,7 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>75</v>
@@ -1594,7 +1591,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>20</v>
@@ -1602,13 +1599,13 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>75</v>
@@ -1625,7 +1622,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="8"/>
       <c r="I15" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>20</v>
@@ -1633,13 +1630,13 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>75</v>
@@ -1656,7 +1653,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="8"/>
       <c r="I16" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>20</v>
@@ -1664,13 +1661,13 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>75</v>
@@ -1701,7 +1698,7 @@
         <v>13</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1738,13 +1735,13 @@
         <v>13</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>75</v>
@@ -1775,13 +1772,13 @@
         <v>13</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>75</v>
@@ -1812,13 +1809,13 @@
         <v>13</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>75</v>
@@ -1849,13 +1846,13 @@
         <v>13</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>75</v>
@@ -1886,13 +1883,13 @@
         <v>13</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>75</v>
@@ -1923,13 +1920,13 @@
         <v>13</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>75</v>
@@ -1960,13 +1957,13 @@
         <v>13</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>75</v>
@@ -1997,13 +1994,13 @@
         <v>13</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>75</v>
@@ -2034,13 +2031,13 @@
         <v>13</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>75</v>
@@ -2065,13 +2062,13 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>75</v>
@@ -2102,13 +2099,13 @@
         <v>13</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>75</v>
@@ -2139,13 +2136,13 @@
         <v>13</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>75</v>
@@ -2164,7 +2161,7 @@
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>27</v>
@@ -2176,13 +2173,13 @@
         <v>13</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>75</v>
@@ -2213,13 +2210,13 @@
         <v>13</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>75</v>
@@ -2250,13 +2247,13 @@
         <v>13</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>75</v>
@@ -2287,7 +2284,7 @@
         <v>13</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2572,7 +2569,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fragen "Kinderbetreuung": Diverse kleine Änderungen in Absprache mit Myriel&Caroline
</commit_message>
<xml_diff>
--- a/inst/shiny-apps/vsim/data/vsim_question_lists_kinderbetreuung.xlsx
+++ b/inst/shiny-apps/vsim/data/vsim_question_lists_kinderbetreuung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianschmid/Documents/R/vsim/inst/shiny-apps/vsim/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE01E6E0-F8CF-514A-BCB1-17CCF693B719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F04A798-A783-A24D-A2F1-73F0E4A18B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{CC769E72-D120-46FE-9FA6-BDE4E08E04F5}"/>
   </bookViews>
   <sheets>
     <sheet name="QAGlist_Teil1" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Qlist_Teil2c" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_4" localSheetId="0" hidden="1">QAGlist_Teil1!$A$1:$G$33</definedName>
+    <definedName name="ExterneDaten_4" localSheetId="0" hidden="1">QAGlist_Teil1!$A$1:$G$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="148">
   <si>
     <t>Qnum</t>
   </si>
@@ -434,9 +434,6 @@
     <t>Finden Sie es in Ordnung, wie viel Zeit Sie pro Woche für die Kinderbetreuung im engeren Sinne (Hausaufgaben erledigen, Essen zubereiten etc.) aufwenden?</t>
   </si>
   <si>
-    <t>Ich fühle mich in meiner Arbeit wertgeschätzt durch meine Kolleg_innen, Vorgesetzten und die Firmenleitung</t>
-  </si>
-  <si>
     <t>Ich bin zufrieden mit meinen aktuellen Möglichkeiten zur Karriereentwicklung.</t>
   </si>
   <si>
@@ -455,12 +452,6 @@
     <t>Ich fühle mich belastet, weil ich während der Arbeit oft auch privaten Verpflichtungen nachkommen muss</t>
   </si>
   <si>
-    <t xml:space="preserve">Ich fühle mich belastet, weil ich zu Hause oft auch beruflichen Verpflichtungen nachkommen muss.  </t>
-  </si>
-  <si>
-    <t>Ich fühle mich belastet, weil ich ausserhalb meiner Arbeitszeit oft auch beruflichen Verpflichtungen nachkommen muss und deshalb zu wenig Zeit für andere Tätigkeiten habe.</t>
-  </si>
-  <si>
     <t>Ich fühle mich während des Home Office belastet, weil oft private Aufgaben dazwischen kommen.</t>
   </si>
   <si>
@@ -486,6 +477,12 @@
   </si>
   <si>
     <t>Finden Sie es in Ordnung, wie viel Zeit Sie pro Woche für Hausarbeiten (wie Putzen, Kochen, Reparieren, Gartenarbeit, Zahlungen, Einkaufen, Waschen etc.) aufwenden?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich fühle mich belastet, weil ich ausserhalb meiner Arbeitszeit oft auch beruflichen Verpflichtungen nachkommen muss.  </t>
+  </si>
+  <si>
+    <t>Ich fühle mich in meiner Arbeit wertgeschätzt durch meine Kolleg_innen, Vorgesetzten und die Firmenleitung.</t>
   </si>
 </sst>
 </file>
@@ -726,8 +723,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9A4626D1-B7A1-4A0E-9ABD-F1802EEF4B4A}" name="Qlist_Teil1" displayName="Qlist_Teil1" ref="A1:M33" totalsRowShown="0">
-  <autoFilter ref="A1:M33" xr:uid="{63A3C723-9C80-47B3-B07E-C2015D435A2D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9A4626D1-B7A1-4A0E-9ABD-F1802EEF4B4A}" name="Qlist_Teil1" displayName="Qlist_Teil1" ref="A1:M32" totalsRowShown="0">
+  <autoFilter ref="A1:M32" xr:uid="{63A3C723-9C80-47B3-B07E-C2015D435A2D}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{6833DAB1-3042-428C-936F-D4BF6D9DD972}" name="Qnum" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{68ACE6E4-2458-484E-B5F0-6043D861F09A}" name="Question" dataDxfId="21"/>
@@ -1084,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F2727F-E159-4B39-B30A-A10ACC8F5533}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1097,7 @@
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="9" width="41.83203125" customWidth="1"/>
+    <col min="9" max="9" width="69" customWidth="1"/>
     <col min="10" max="10" width="70.5" customWidth="1"/>
     <col min="11" max="12" width="10.83203125" customWidth="1"/>
     <col min="13" max="13" width="14.5" customWidth="1"/>
@@ -1150,7 +1147,7 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>71</v>
@@ -1183,7 +1180,7 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>71</v>
@@ -1605,7 +1602,7 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>75</v>
@@ -1667,7 +1664,7 @@
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>75</v>
@@ -1741,7 +1738,7 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>75</v>
@@ -1815,7 +1812,7 @@
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>75</v>
@@ -1852,7 +1849,7 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>75</v>
@@ -1889,7 +1886,7 @@
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>75</v>
@@ -1926,7 +1923,7 @@
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>75</v>
@@ -1963,7 +1960,7 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>75</v>
@@ -2000,7 +1997,7 @@
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>75</v>
@@ -2014,30 +2011,24 @@
       <c r="F26" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="G26" s="3"/>
       <c r="H26" s="8"/>
       <c r="I26" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
       <c r="M26" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>75</v>
@@ -2051,24 +2042,30 @@
       <c r="F27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H27" s="8"/>
       <c r="I27" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
+      <c r="K27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="M27" s="6" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>75</v>
@@ -2087,7 +2084,7 @@
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>27</v>
@@ -2099,13 +2096,13 @@
         <v>13</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>75</v>
@@ -2124,7 +2121,7 @@
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="5" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>27</v>
@@ -2136,13 +2133,13 @@
         <v>13</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>75</v>
@@ -2161,7 +2158,7 @@
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="5" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>27</v>
@@ -2173,13 +2170,13 @@
         <v>13</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>75</v>
@@ -2198,7 +2195,7 @@
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>27</v>
@@ -2216,7 +2213,7 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>75</v>
@@ -2235,7 +2232,7 @@
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>27</v>
@@ -2247,43 +2244,6 @@
         <v>13</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="8"/>
-      <c r="I33" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M33" s="6" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>